<commit_message>
add assignment volume function
</commit_message>
<xml_diff>
--- a/piu_statistics.xlsx
+++ b/piu_statistics.xlsx
@@ -14,9 +14,9 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="9">
   <si>
-    <t>Period</t>
+    <t>Name</t>
   </si>
   <si>
     <t>上周</t>
@@ -354,6 +354,264 @@
 </c:chartSpace>
 </file>
 
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:lang val="en-US"/>
+  <c:style val="1"/>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>制造协同周任务量分析表</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+    </c:title>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$K$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>上周</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln>
+              <a:solidFill>
+                <a:srgbClr val="FFFF00"/>
+              </a:solidFill>
+            </a:ln>
+          </c:spPr>
+          <c:cat>
+            <c:strRef>
+              <c:f>Sheet1!$J2:$J7</c:f>
+              <c:strCache>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>罗远明</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>刘兴国</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>王超</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>王言章</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>李若愚</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>聂正</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$K2:$K7</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>9</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$L$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>本周</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln>
+              <a:solidFill>
+                <a:srgbClr val="800080"/>
+              </a:solidFill>
+            </a:ln>
+          </c:spPr>
+          <c:cat>
+            <c:strRef>
+              <c:f>Sheet1!$J2:$J7</c:f>
+              <c:strCache>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>罗远明</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>刘兴国</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>王超</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>王言章</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>李若愚</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>聂正</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$L2:$L7</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:axId val="50020001"/>
+        <c:axId val="50020002"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="50020001"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Member name</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+        </c:title>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="50020002"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="50020002"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Weekly code volume data</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="50020001"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout/>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
@@ -381,6 +639,36 @@
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>9</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>304800</xdr:colOff>
+      <xdr:row>23</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="3" name="Chart 2"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -674,13 +962,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C7"/>
+  <dimension ref="A1:L7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:3">
+    <row r="1" spans="1:12">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -690,8 +978,17 @@
       <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
+      <c r="J1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>2</v>
+      </c>
     </row>
-    <row r="2" spans="1:3">
+    <row r="2" spans="1:12">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -701,8 +998,17 @@
       <c r="C2">
         <v>1431</v>
       </c>
+      <c r="J2" t="s">
+        <v>3</v>
+      </c>
+      <c r="K2">
+        <v>0</v>
+      </c>
+      <c r="L2">
+        <v>1</v>
+      </c>
     </row>
-    <row r="3" spans="1:3">
+    <row r="3" spans="1:12">
       <c r="A3" t="s">
         <v>4</v>
       </c>
@@ -712,8 +1018,17 @@
       <c r="C3">
         <v>2228</v>
       </c>
+      <c r="J3" t="s">
+        <v>4</v>
+      </c>
+      <c r="K3">
+        <v>1</v>
+      </c>
+      <c r="L3">
+        <v>0</v>
+      </c>
     </row>
-    <row r="4" spans="1:3">
+    <row r="4" spans="1:12">
       <c r="A4" t="s">
         <v>5</v>
       </c>
@@ -723,8 +1038,17 @@
       <c r="C4">
         <v>1686</v>
       </c>
+      <c r="J4" t="s">
+        <v>5</v>
+      </c>
+      <c r="K4">
+        <v>8</v>
+      </c>
+      <c r="L4">
+        <v>1</v>
+      </c>
     </row>
-    <row r="5" spans="1:3">
+    <row r="5" spans="1:12">
       <c r="A5" t="s">
         <v>6</v>
       </c>
@@ -734,8 +1058,17 @@
       <c r="C5">
         <v>1849</v>
       </c>
+      <c r="J5" t="s">
+        <v>6</v>
+      </c>
+      <c r="K5">
+        <v>2</v>
+      </c>
+      <c r="L5">
+        <v>3</v>
+      </c>
     </row>
-    <row r="6" spans="1:3">
+    <row r="6" spans="1:12">
       <c r="A6" t="s">
         <v>7</v>
       </c>
@@ -745,8 +1078,17 @@
       <c r="C6">
         <v>14619</v>
       </c>
+      <c r="J6" t="s">
+        <v>7</v>
+      </c>
+      <c r="K6">
+        <v>5</v>
+      </c>
+      <c r="L6">
+        <v>4</v>
+      </c>
     </row>
-    <row r="7" spans="1:3">
+    <row r="7" spans="1:12">
       <c r="A7" t="s">
         <v>8</v>
       </c>
@@ -755,6 +1097,15 @@
       </c>
       <c r="C7">
         <v>531</v>
+      </c>
+      <c r="J7" t="s">
+        <v>8</v>
+      </c>
+      <c r="K7">
+        <v>9</v>
+      </c>
+      <c r="L7">
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>